<commit_message>
refactor + add evaluation_notebook.ipynb
</commit_message>
<xml_diff>
--- a/additional_experiments/experiment_tasks.xlsx
+++ b/additional_experiments/experiment_tasks.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ozzafar\LINX\additional_experiments\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{33706DA8-1F91-44FE-9C6E-DBBA69BB92EC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{087290C6-30E7-49DB-9958-C2C6AFF71B30}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-38520" yWindow="-2340" windowWidth="38640" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="6090" yWindow="2295" windowWidth="25560" windowHeight="11145" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -447,8 +447,8 @@
   </sheetPr>
   <dimension ref="A1:X807"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C20" sqref="C20"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>

</xml_diff>